<commit_message>
fixed bugs and allowed content to any URL
</commit_message>
<xml_diff>
--- a/timeWarpVT - template.xlsx
+++ b/timeWarpVT - template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob.Durell\code\timewarpvt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BCEBAE-9E08-4805-A793-93FA8C851208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E2042D-D68C-4CE2-A43D-058FE5881268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D14AF042-F5BD-4880-B7CD-563BC1FF5D38}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="172">
   <si>
     <t>EASTRAT</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>Desc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>line end char</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +584,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,14 +715,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -724,7 +730,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -748,13 +772,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>380999</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -829,14 +853,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>137881</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>381643</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>400693</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
@@ -873,13 +897,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>52388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -928,13 +952,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>323851</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -1004,13 +1028,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>628649</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>185738</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -1063,7 +1087,7 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>66674</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
@@ -1437,10 +1461,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504A1DCA-A754-49FE-8C75-531927B90C22}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:Q17"/>
+  <dimension ref="B2:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,11 +1472,13 @@
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="17" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="16" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1460,89 +1486,89 @@
         <v>12</v>
       </c>
       <c r="D2" s="4">
+        <v>44717</v>
+      </c>
+      <c r="E2" s="4">
         <v>44718</v>
       </c>
-      <c r="E2" s="4">
-        <f>D2+1</f>
+      <c r="F2" s="4">
+        <f>E2+1</f>
         <v>44719</v>
       </c>
-      <c r="F2" s="4">
-        <f t="shared" ref="F2" si="0">E2+1</f>
+      <c r="G2" s="4">
+        <f t="shared" ref="G2" si="0">F2+1</f>
         <v>44720</v>
       </c>
-      <c r="G2" s="4">
-        <f t="shared" ref="G2" si="1">F2+1</f>
+      <c r="H2" s="4">
+        <f t="shared" ref="H2" si="1">G2+1</f>
         <v>44721</v>
       </c>
-      <c r="H2" s="4">
-        <f t="shared" ref="H2" si="2">G2+1</f>
+      <c r="I2" s="4">
+        <f t="shared" ref="I2" si="2">H2+1</f>
         <v>44722</v>
       </c>
-      <c r="I2" s="4">
-        <f t="shared" ref="I2" si="3">H2+1</f>
+      <c r="J2" s="4">
+        <f t="shared" ref="J2" si="3">I2+1</f>
         <v>44723</v>
       </c>
-      <c r="J2" s="4">
-        <f t="shared" ref="J2" si="4">I2+1</f>
+      <c r="K2" s="4">
+        <f t="shared" ref="K2" si="4">J2+1</f>
         <v>44724</v>
       </c>
-      <c r="K2" s="4">
-        <f t="shared" ref="K2" si="5">J2+1</f>
+      <c r="L2" s="4">
+        <f t="shared" ref="L2" si="5">K2+1</f>
         <v>44725</v>
       </c>
-      <c r="L2" s="4">
-        <f t="shared" ref="L2" si="6">K2+1</f>
+      <c r="M2" s="4">
+        <f t="shared" ref="M2" si="6">L2+1</f>
         <v>44726</v>
       </c>
-      <c r="M2" s="4">
-        <f t="shared" ref="M2" si="7">L2+1</f>
+      <c r="N2" s="4">
+        <f t="shared" ref="N2" si="7">M2+1</f>
         <v>44727</v>
       </c>
-      <c r="N2" s="4">
-        <f t="shared" ref="N2" si="8">M2+1</f>
+      <c r="O2" s="4">
+        <f t="shared" ref="O2" si="8">N2+1</f>
         <v>44728</v>
       </c>
-      <c r="O2" s="4">
-        <f t="shared" ref="O2" si="9">N2+1</f>
+      <c r="P2" s="4">
+        <f t="shared" ref="P2" si="9">O2+1</f>
         <v>44729</v>
       </c>
-      <c r="P2" s="4">
-        <f t="shared" ref="P2" si="10">O2+1</f>
+      <c r="Q2" s="4">
+        <f>P2+1</f>
         <v>44730</v>
       </c>
-      <c r="Q2" s="4">
-        <f t="shared" ref="Q2" si="11">P2+1</f>
-        <v>44731</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R2" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>123</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="19"/>
+      <c r="E3" s="8">
         <v>2.5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8">
         <v>0.5</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="9"/>
-      <c r="K3" s="8">
+      <c r="K3" s="9"/>
+      <c r="L3" s="8">
         <v>1.5</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>2</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0.5</v>
       </c>
       <c r="N3" s="8">
         <v>0.5</v>
@@ -1550,410 +1576,454 @@
       <c r="O3" s="8">
         <v>0.5</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="P3" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="5">
+      <c r="K4" s="6"/>
+      <c r="L4" s="5">
         <v>2</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>1.5</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>0.5</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>3</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>0.5</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>1</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="12"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5">
+      <c r="D6" s="20"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5">
         <v>1.5</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="5">
+      <c r="K6" s="6"/>
+      <c r="L6" s="5">
         <v>1</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5">
+      <c r="M6" s="5"/>
+      <c r="N6" s="5">
         <v>1</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5">
+      <c r="O6" s="5"/>
+      <c r="P6" s="5">
         <v>0.5</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="Q6" s="6"/>
+      <c r="R6" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5">
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5">
         <v>1</v>
       </c>
-      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="12"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="P7" s="5"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="20"/>
+      <c r="E8" s="5">
         <v>0.5</v>
       </c>
-      <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="5">
         <v>0.5</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="5">
+        <v>0.5</v>
+      </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="5">
+      <c r="K8" s="6"/>
+      <c r="L8" s="5">
         <v>0.5</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5">
+      <c r="M8" s="5"/>
+      <c r="N8" s="5">
         <v>1</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0.5</v>
       </c>
       <c r="O8" s="5">
         <v>0.5</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="12"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="P8" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="5">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5">
         <v>3.5</v>
       </c>
-      <c r="O9" s="5"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="12"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="20"/>
+      <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5">
-        <v>1.5</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5">
         <v>1.5</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="5">
+        <v>1.5</v>
+      </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="5">
+      <c r="K10" s="6"/>
+      <c r="L10" s="5">
         <v>1</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="M10" s="5"/>
       <c r="N10" s="5">
         <v>0.5</v>
       </c>
       <c r="O10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="5">
         <v>1</v>
       </c>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="Q10" s="6"/>
+      <c r="R10" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="5">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5">
         <v>7</v>
       </c>
-      <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="P11" s="5"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>123</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="5">
-        <v>4</v>
-      </c>
+      <c r="D12" s="20"/>
       <c r="E12" s="5">
         <v>4</v>
       </c>
       <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
         <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>4</v>
       </c>
       <c r="H12" s="5">
         <v>4</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="5">
+        <v>4</v>
+      </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="5">
+      <c r="K12" s="6"/>
+      <c r="L12" s="5">
         <v>2</v>
       </c>
-      <c r="L12" s="5">
+      <c r="M12" s="5">
         <v>3.5</v>
       </c>
-      <c r="M12" s="5">
+      <c r="N12" s="5">
         <v>4.5</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5">
+      <c r="O12" s="5"/>
+      <c r="P12" s="5">
         <v>4</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="12"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="5"/>
+      <c r="K13" s="6"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="12"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="12"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="6"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="12"/>
-    </row>
-    <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="17"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="18" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="17" spans="4:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f>SUM(D3:D16)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" ref="D17:P17" si="10">SUM(E3:E16)</f>
         <v>8</v>
       </c>
-      <c r="E17" s="2">
-        <f>SUM(E3:E16)</f>
+      <c r="F17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="F17" s="2">
-        <f>SUM(F3:F16)</f>
+      <c r="G17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="G17" s="2">
-        <f>SUM(G3:G16)</f>
+      <c r="H17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="H17" s="2">
-        <f>SUM(H3:H16)</f>
+      <c r="I17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="I17" s="2">
-        <f>SUM(I3:I16)</f>
+      <c r="J17" s="2">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J17" s="2">
-        <f>SUM(J3:J16)</f>
+      <c r="K17" s="2">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K17" s="2">
-        <f>SUM(K3:K16)</f>
+      <c r="L17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="L17" s="2">
-        <f>SUM(L3:L16)</f>
+      <c r="M17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="M17" s="2">
-        <f>SUM(M3:M16)</f>
+      <c r="N17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="N17" s="2">
-        <f>SUM(N3:N16)</f>
+      <c r="O17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="O17" s="2">
-        <f>SUM(O3:O16)</f>
+      <c r="P17" s="2">
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="P17" s="2">
-        <f t="shared" ref="P17:Q17" si="12">SUM(P3:P16)</f>
-        <v>0</v>
-      </c>
       <c r="Q17" s="2">
-        <f t="shared" si="12"/>
+        <f>SUM(Q3:Q16)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>